<commit_message>
Add link to prevention pdf in excel
</commit_message>
<xml_diff>
--- a/Voorbereiding + aanwezigheden Aanwezigheden.xlsx
+++ b/Voorbereiding + aanwezigheden Aanwezigheden.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/912478989d4531eb/Louis Vanden Borre/Macbook Pro Louis/Hockey/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Desktop\Programming\IndianaH2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{108FCCCE-5B2B-4A54-9EF3-018364C3E600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D9862F-B809-42E2-9D44-6AF55601FCCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="500" windowWidth="25920" windowHeight="13180" xr2:uid="{FC8ADF5B-421C-7E47-AE77-8248CE5A8B0F}"/>
+    <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{FC8ADF5B-421C-7E47-AE77-8248CE5A8B0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Fysiek" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="52">
   <si>
     <t>Week 1</t>
   </si>
@@ -188,13 +188,16 @@
   </si>
   <si>
     <t>arthur</t>
+  </si>
+  <si>
+    <t>Prevention PDF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -204,6 +207,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -407,10 +418,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -427,7 +439,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -437,15 +458,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -466,11 +478,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -785,18 +799,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543FB4E3-B3E9-4D4C-AE34-53475CE761B5}">
   <dimension ref="A1:BS30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E17" sqref="E17"/>
       <selection activeCell="A22" sqref="A22"/>
+      <selection pane="topRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.125" customWidth="1"/>
+    <col min="1" max="1" width="12.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71">
+    <row r="1" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
       <c r="B1" s="26" t="s">
         <v>0</v>
@@ -889,7 +903,7 @@
       <c r="BR1" s="27"/>
       <c r="BS1" s="28"/>
     </row>
-    <row r="2" spans="1:71">
+    <row r="2" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -936,7 +950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:71">
+    <row r="3" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -963,7 +977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:71">
+    <row r="4" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -988,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:71">
+    <row r="5" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -1013,7 +1027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:71">
+    <row r="6" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1038,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:71">
+    <row r="7" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -1063,7 +1077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:71">
+    <row r="8" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -1090,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:71">
+    <row r="9" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -1115,7 +1129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:71">
+    <row r="10" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -1140,7 +1154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:71">
+    <row r="11" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1165,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:71">
+    <row r="12" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -1190,7 +1204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:71">
+    <row r="13" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
@@ -1227,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:71">
+    <row r="14" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
@@ -1252,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:71">
+    <row r="15" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -1279,7 +1293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:71">
+    <row r="16" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1304,7 +1318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:71">
+    <row r="17" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -1331,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:71">
+    <row r="18" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>37</v>
       </c>
@@ -1356,99 +1370,99 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:71">
-      <c r="B22" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="20" t="s">
+    <row r="22" spans="1:71" x14ac:dyDescent="0.3">
+      <c r="B22" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="20" t="s">
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="22"/>
-      <c r="W22" s="20" t="s">
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="17"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="18"/>
+      <c r="W22" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="X22" s="21"/>
-      <c r="Y22" s="21"/>
-      <c r="Z22" s="21"/>
-      <c r="AA22" s="21"/>
-      <c r="AB22" s="21"/>
-      <c r="AC22" s="22"/>
-      <c r="AD22" s="20" t="s">
+      <c r="X22" s="17"/>
+      <c r="Y22" s="17"/>
+      <c r="Z22" s="17"/>
+      <c r="AA22" s="17"/>
+      <c r="AB22" s="17"/>
+      <c r="AC22" s="18"/>
+      <c r="AD22" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="AE22" s="21"/>
-      <c r="AF22" s="21"/>
-      <c r="AG22" s="21"/>
-      <c r="AH22" s="21"/>
-      <c r="AI22" s="21"/>
-      <c r="AJ22" s="22"/>
-      <c r="AK22" s="20" t="s">
+      <c r="AE22" s="17"/>
+      <c r="AF22" s="17"/>
+      <c r="AG22" s="17"/>
+      <c r="AH22" s="17"/>
+      <c r="AI22" s="17"/>
+      <c r="AJ22" s="18"/>
+      <c r="AK22" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="AL22" s="21"/>
-      <c r="AM22" s="21"/>
-      <c r="AN22" s="21"/>
-      <c r="AO22" s="21"/>
-      <c r="AP22" s="21"/>
-      <c r="AQ22" s="22"/>
-      <c r="AR22" s="20" t="s">
+      <c r="AL22" s="17"/>
+      <c r="AM22" s="17"/>
+      <c r="AN22" s="17"/>
+      <c r="AO22" s="17"/>
+      <c r="AP22" s="17"/>
+      <c r="AQ22" s="18"/>
+      <c r="AR22" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="AS22" s="21"/>
-      <c r="AT22" s="21"/>
-      <c r="AU22" s="21"/>
-      <c r="AV22" s="21"/>
-      <c r="AW22" s="21"/>
-      <c r="AX22" s="22"/>
-      <c r="AY22" s="20" t="s">
+      <c r="AS22" s="17"/>
+      <c r="AT22" s="17"/>
+      <c r="AU22" s="17"/>
+      <c r="AV22" s="17"/>
+      <c r="AW22" s="17"/>
+      <c r="AX22" s="18"/>
+      <c r="AY22" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="AZ22" s="21"/>
-      <c r="BA22" s="21"/>
-      <c r="BB22" s="21"/>
-      <c r="BC22" s="21"/>
-      <c r="BD22" s="21"/>
-      <c r="BE22" s="22"/>
-      <c r="BF22" s="20" t="s">
+      <c r="AZ22" s="17"/>
+      <c r="BA22" s="17"/>
+      <c r="BB22" s="17"/>
+      <c r="BC22" s="17"/>
+      <c r="BD22" s="17"/>
+      <c r="BE22" s="18"/>
+      <c r="BF22" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="BG22" s="21"/>
-      <c r="BH22" s="21"/>
-      <c r="BI22" s="21"/>
-      <c r="BJ22" s="21"/>
-      <c r="BK22" s="21"/>
-      <c r="BL22" s="22"/>
-      <c r="BM22" s="20" t="s">
+      <c r="BG22" s="17"/>
+      <c r="BH22" s="17"/>
+      <c r="BI22" s="17"/>
+      <c r="BJ22" s="17"/>
+      <c r="BK22" s="17"/>
+      <c r="BL22" s="18"/>
+      <c r="BM22" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="BN22" s="21"/>
-      <c r="BO22" s="21"/>
-      <c r="BP22" s="21"/>
-      <c r="BQ22" s="21"/>
-      <c r="BR22" s="21"/>
-      <c r="BS22" s="22"/>
-    </row>
-    <row r="23" spans="1:71">
+      <c r="BN22" s="17"/>
+      <c r="BO22" s="17"/>
+      <c r="BP22" s="17"/>
+      <c r="BQ22" s="17"/>
+      <c r="BR22" s="17"/>
+      <c r="BS22" s="18"/>
+    </row>
+    <row r="23" spans="1:71" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
         <v>38</v>
       </c>
@@ -1476,187 +1490,204 @@
       <c r="N23" s="24"/>
       <c r="O23" s="25"/>
     </row>
-    <row r="24" spans="1:71">
+    <row r="24" spans="1:71" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
         <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="17"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="20"/>
       <c r="I24" s="1">
         <v>1</v>
       </c>
       <c r="J24" t="s">
         <v>41</v>
       </c>
-      <c r="K24" s="29" t="s">
+      <c r="K24" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="17"/>
-    </row>
-    <row r="25" spans="1:71" ht="15.95" customHeight="1">
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="20"/>
+    </row>
+    <row r="25" spans="1:71" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="17"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="1">
         <v>2</v>
       </c>
       <c r="J25" t="s">
         <v>41</v>
       </c>
-      <c r="K25" s="29" t="s">
+      <c r="K25" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="17"/>
-    </row>
-    <row r="26" spans="1:71" ht="15.95" customHeight="1">
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="20"/>
+    </row>
+    <row r="26" spans="1:71" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="17"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="1">
         <v>3</v>
       </c>
       <c r="J26" t="s">
         <v>41</v>
       </c>
-      <c r="K26" s="29" t="s">
+      <c r="K26" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="29"/>
-      <c r="O26" s="17"/>
-    </row>
-    <row r="27" spans="1:71" ht="15.95" customHeight="1">
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="20"/>
+    </row>
+    <row r="27" spans="1:71" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
         <v>4</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="17"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="20"/>
       <c r="I27" s="1">
         <v>4</v>
       </c>
       <c r="J27" t="s">
         <v>43</v>
       </c>
-      <c r="K27" s="29" t="s">
+      <c r="K27" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="17"/>
-    </row>
-    <row r="28" spans="1:71">
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="20"/>
+    </row>
+    <row r="28" spans="1:71" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
         <v>5</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="17"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="1">
         <v>5</v>
       </c>
       <c r="J28" t="s">
         <v>43</v>
       </c>
-      <c r="K28" s="29" t="s">
+      <c r="K28" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="17"/>
-    </row>
-    <row r="29" spans="1:71">
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="20"/>
+    </row>
+    <row r="29" spans="1:71" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="4">
         <v>6</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="19"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="22"/>
       <c r="I29" s="4">
         <v>6</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="K29" s="18" t="s">
+      <c r="K29" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="19"/>
-    </row>
-    <row r="30" spans="1:71">
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="22"/>
+    </row>
+    <row r="30" spans="1:71" x14ac:dyDescent="0.3">
+      <c r="B30" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="30"/>
       <c r="E30" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="BM22:BS22"/>
-    <mergeCell ref="AD22:AJ22"/>
-    <mergeCell ref="AK22:AQ22"/>
-    <mergeCell ref="AR22:AX22"/>
-    <mergeCell ref="AY22:BE22"/>
-    <mergeCell ref="BF22:BL22"/>
+  <mergeCells count="35">
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="BM1:BS1"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AC1"/>
+    <mergeCell ref="AD1:AJ1"/>
+    <mergeCell ref="AK1:AQ1"/>
+    <mergeCell ref="AR1:AX1"/>
+    <mergeCell ref="AY1:BE1"/>
+    <mergeCell ref="BF1:BL1"/>
     <mergeCell ref="K27:O27"/>
     <mergeCell ref="K28:O28"/>
     <mergeCell ref="K29:O29"/>
@@ -1667,24 +1698,12 @@
     <mergeCell ref="K24:O24"/>
     <mergeCell ref="K25:O25"/>
     <mergeCell ref="K26:O26"/>
-    <mergeCell ref="BM1:BS1"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AC1"/>
-    <mergeCell ref="AD1:AJ1"/>
-    <mergeCell ref="AK1:AQ1"/>
-    <mergeCell ref="AR1:AX1"/>
-    <mergeCell ref="AY1:BE1"/>
-    <mergeCell ref="BF1:BL1"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="BM22:BS22"/>
+    <mergeCell ref="AD22:AJ22"/>
+    <mergeCell ref="AK22:AQ22"/>
+    <mergeCell ref="AR22:AX22"/>
+    <mergeCell ref="AY22:BE22"/>
+    <mergeCell ref="BF22:BL22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
@@ -1692,6 +1711,9 @@
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B30:C30" r:id="rId1" display="Prevention PDF" xr:uid="{1385760F-9856-4CF6-A706-630E38B636B8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1704,9 +1726,9 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" thickBot="1">
+    <row r="1" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7"/>
       <c r="B1" s="26" t="s">
         <v>0</v>
@@ -1737,7 +1759,7 @@
       <c r="T1" s="27"/>
       <c r="U1" s="28"/>
     </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1">
+    <row r="2" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
@@ -1802,7 +1824,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>21</v>
       </c>
@@ -1863,7 +1885,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>23</v>
       </c>
@@ -1900,7 +1922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
@@ -1937,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>25</v>
       </c>
@@ -1974,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>26</v>
       </c>
@@ -2011,7 +2033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>27</v>
       </c>
@@ -2048,7 +2070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>28</v>
       </c>
@@ -2085,7 +2107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>29</v>
       </c>
@@ -2122,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>30</v>
       </c>
@@ -2159,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>31</v>
       </c>
@@ -2196,7 +2218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>32</v>
       </c>
@@ -2233,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>33</v>
       </c>
@@ -2270,7 +2292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>34</v>
       </c>
@@ -2307,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>35</v>
       </c>
@@ -2344,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>50</v>
       </c>
@@ -2381,7 +2403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15.75" thickBot="1">
+    <row r="18" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>37</v>
       </c>

</xml_diff>